<commit_message>
New gem 'bullet' installed.
</commit_message>
<xml_diff>
--- a/要件定義書(ポートフォリオ).xlsx
+++ b/要件定義書(ポートフォリオ).xlsx
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="532" uniqueCount="298">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="537" uniqueCount="298">
   <si>
     <t>●アイディアの概要</t>
   </si>
@@ -2640,7 +2640,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -2735,6 +2735,14 @@
       <color rgb="FFE3E3E3"/>
       <name val="Consolas"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Yu Gothic"/>
+      <family val="3"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -2851,7 +2859,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2901,8 +2909,12 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="80">
+  <cellXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3111,8 +3123,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="49">
+  <cellStyles count="53">
     <cellStyle name="ハイパーリンク" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="ハイパーリンク" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="ハイパーリンク" xfId="5" builtinId="8" hidden="1"/>
@@ -3137,6 +3152,8 @@
     <cellStyle name="ハイパーリンク" xfId="43" builtinId="8" hidden="1"/>
     <cellStyle name="ハイパーリンク" xfId="45" builtinId="8" hidden="1"/>
     <cellStyle name="ハイパーリンク" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="51" builtinId="8" hidden="1"/>
     <cellStyle name="標準" xfId="0" builtinId="0"/>
     <cellStyle name="表示済みのハイパーリンク" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="表示済みのハイパーリンク" xfId="4" builtinId="9" hidden="1"/>
@@ -3162,6 +3179,8 @@
     <cellStyle name="表示済みのハイパーリンク" xfId="44" builtinId="9" hidden="1"/>
     <cellStyle name="表示済みのハイパーリンク" xfId="46" builtinId="9" hidden="1"/>
     <cellStyle name="表示済みのハイパーリンク" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="52" builtinId="9" hidden="1"/>
   </cellStyles>
   <dxfs count="18">
     <dxf>
@@ -27508,8 +27527,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="85" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView tabSelected="1" zoomScale="85" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultRowHeight="20" x14ac:dyDescent="0.3"/>
@@ -27790,8 +27809,8 @@
       <c r="I12" s="51" t="s">
         <v>5</v>
       </c>
-      <c r="J12" s="79" t="s">
-        <v>45</v>
+      <c r="J12" s="80" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="40" x14ac:dyDescent="0.3">
@@ -27824,6 +27843,9 @@
       <c r="I13" s="51" t="s">
         <v>5</v>
       </c>
+      <c r="J13" s="80" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="44">
@@ -27855,6 +27877,9 @@
       <c r="I14" s="51" t="s">
         <v>143</v>
       </c>
+      <c r="J14" s="80" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="44">
@@ -27921,8 +27946,11 @@
       <c r="I16" s="51" t="s">
         <v>5</v>
       </c>
+      <c r="J16" s="80" t="s">
+        <v>34</v>
+      </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" s="44">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -27951,7 +27979,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" s="44">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -27980,7 +28008,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" s="44">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -28010,8 +28038,11 @@
       <c r="I19" s="51" t="s">
         <v>5</v>
       </c>
+      <c r="J19" s="80" t="s">
+        <v>34</v>
+      </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" s="44">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -28041,8 +28072,11 @@
       <c r="I20" s="51" t="s">
         <v>5</v>
       </c>
+      <c r="J20" s="80" t="s">
+        <v>34</v>
+      </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" s="44">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -28071,7 +28105,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" s="44">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -28100,7 +28134,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23" s="44">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -28129,7 +28163,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24" s="44">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -28158,7 +28192,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25" s="44">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -28187,7 +28221,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26" s="44">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -28216,7 +28250,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="27" spans="1:9" ht="40" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:10" ht="40" x14ac:dyDescent="0.3">
       <c r="A27" s="44">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -28245,7 +28279,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A28" s="44">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -28274,7 +28308,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A29" s="44">
         <f t="shared" si="0"/>
         <v>23</v>
@@ -28355,11 +28389,6 @@
   </conditionalFormatting>
   <conditionalFormatting sqref="J11">
     <cfRule type="cellIs" dxfId="3" priority="2" operator="greaterThan">
-      <formula>$I$7:$I$25="低"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J12">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="greaterThan">
       <formula>$I$7:$I$25="低"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>